<commit_message>
output of resolving disagreements - in progress
Former-commit-id: 99692a9239cc7a85ef263ff832498fc77dd58329
</commit_message>
<xml_diff>
--- a/Classifications/Vid_1_Morgan_Proofread_Calvin.xlsx
+++ b/Classifications/Vid_1_Morgan_Proofread_Calvin.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/morgandeneve/Documents/_HawCHI/CalvinsClassification/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iowa-my.sharepoint.com/personal/krector_uiowa_edu/Documents/aerobictextreview/Classifications/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C9BA6B64-C06B-1E42-B451-CADF41EFF0DC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="8_{C9BA6B64-C06B-1E42-B451-CADF41EFF0DC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B2E9C343-AAFF-4FBC-A900-215CCE2C591A}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="256">
   <si>
     <t>hey everybody it's your personal trainer coach Kozak here from HASFIT.</t>
   </si>
@@ -291,11 +291,6 @@
     <t>so we got ten seconds</t>
   </si>
   <si>
-    <t>I'm going to grab my dumbbells we're
-getting ready we're starting with the
-row</t>
-  </si>
-  <si>
     <t>so right now
 our backs working but at the same time
 our chest may be resting</t>
@@ -928,6 +923,12 @@
   </si>
   <si>
     <t>the only other equipment that you may want for this workout is a chair or a box</t>
+  </si>
+  <si>
+    <t>I'm going to grab my dumbbells</t>
+  </si>
+  <si>
+    <t>we're getting ready we're starting with the row</t>
   </si>
 </sst>
 </file>
@@ -943,7 +944,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -962,6 +963,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -975,7 +982,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -984,6 +991,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1266,326 +1277,329 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K121"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I6" sqref="I6"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="33.5" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" customWidth="1"/>
-    <col min="5" max="5" width="45.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="3.5" style="2" customWidth="1"/>
-    <col min="7" max="7" width="15.1640625" customWidth="1"/>
-    <col min="8" max="8" width="2.33203125" customWidth="1"/>
-    <col min="9" max="9" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="1.83203125" customWidth="1"/>
-    <col min="11" max="11" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.6328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="33.453125" customWidth="1"/>
+    <col min="4" max="4" width="8.6328125" customWidth="1"/>
+    <col min="5" max="5" width="45.453125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="3.453125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="15.1796875" customWidth="1"/>
+    <col min="8" max="8" width="2.36328125" customWidth="1"/>
+    <col min="9" max="9" width="24.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="1.81640625" customWidth="1"/>
+    <col min="11" max="11" width="35.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D1" t="s">
         <v>6</v>
       </c>
       <c r="E1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G1" t="s">
+        <v>144</v>
+      </c>
+      <c r="I1" t="s">
         <v>145</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>146</v>
       </c>
-      <c r="K1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+        <v>139</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C3" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="87" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="I4" t="s">
+        <v>140</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="I4" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="E5" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="I5" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="80" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="I6" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="48" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>132</v>
-      </c>
       <c r="C8" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="87" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="80" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="96" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="48" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>139</v>
-      </c>
       <c r="C11" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="I11" s="4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="I12" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="I12" s="4" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="C14" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="C15" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="C18" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="I13" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="48" x14ac:dyDescent="0.2">
-      <c r="C14" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="C15" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C16" s="1" t="s">
+    </row>
+    <row r="19" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E20" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E21" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="C18" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="E20" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="E21" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>118</v>
-      </c>
       <c r="E22" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="E24" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>62</v>
       </c>
@@ -1593,7 +1607,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>40</v>
       </c>
@@ -1601,7 +1615,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>36</v>
       </c>
@@ -1609,7 +1623,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>20</v>
       </c>
@@ -1617,36 +1631,36 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>2</v>
       </c>
@@ -1654,23 +1668,23 @@
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>1</v>
       </c>
@@ -1678,136 +1692,136 @@
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E40" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="E41" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="E41" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="E42" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A43" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E43" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="E43" s="1" t="s">
+    <row r="44" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A44" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="E44" s="1" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="64" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E45" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="E46" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="E46" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="E51" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>38</v>
       </c>
@@ -1815,44 +1829,44 @@
         <v>31</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="E58" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>41</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>45</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>46</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>47</v>
       </c>
@@ -1860,450 +1874,450 @@
         <v>33</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>51</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="E66" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>53</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
         <v>54</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
         <v>56</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
         <v>55</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
         <v>57</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
         <v>50</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
         <v>58</v>
       </c>
       <c r="E73" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A74" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+      <c r="A75" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="E75" s="1" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A74" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" ht="80" x14ac:dyDescent="0.2">
-      <c r="A75" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="E75" s="1" t="s">
+    <row r="76" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A76" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E76" s="1" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A76" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A79" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A80" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A81" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A82" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A83" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A84" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A85" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A86" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A87" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A88" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A89" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A90" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A91" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A92" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A93" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E93" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E78" s="1" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A79" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A80" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A81" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="E81" s="1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A82" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="E82" s="1" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A83" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" ht="64" x14ac:dyDescent="0.2">
-      <c r="A84" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="E84" s="1" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A85" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A86" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E86" s="1" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A87" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="E87" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A88" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="E88" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A89" s="1" t="s">
+    </row>
+    <row r="94" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A94" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E94" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="E89" s="1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A90" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E90" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A91" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E91" s="1" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A92" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E92" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A93" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E93" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A94" s="1" t="s">
+    </row>
+    <row r="95" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A95" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E94" s="1" t="s">
+      <c r="E95" s="1" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="95" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A95" s="1" t="s">
+    <row r="96" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A96" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E95" s="1" t="s">
+      <c r="E96" s="1" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="96" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A96" s="1" t="s">
+    <row r="97" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A97" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="E96" s="1" t="s">
+      <c r="E97" s="1" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="97" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A97" s="1" t="s">
+    <row r="98" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A98" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E97" s="1" t="s">
+      <c r="E98" s="1" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="98" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A98" s="1" t="s">
+    <row r="99" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A99" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E98" s="1" t="s">
+      <c r="E99" s="1" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="99" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A99" s="1" t="s">
+    <row r="100" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A100" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E99" s="1" t="s">
+      <c r="E100" s="1" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="100" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A100" s="1" t="s">
+    <row r="101" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A101" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E100" s="1" t="s">
+      <c r="E101" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A102" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E102" s="1" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="101" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A101" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E101" s="1" t="s">
+    <row r="103" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A103" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E103" s="1" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="102" spans="1:5" ht="64" x14ac:dyDescent="0.2">
-      <c r="A102" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E102" s="1" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A103" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E103" s="1" t="s">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A104" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E104" s="1" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="104" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A104" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E104" s="1" t="s">
+    <row r="105" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A105" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E105" s="1" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="105" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A105" s="1" t="s">
+    <row r="106" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A106" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E105" s="1" t="s">
+      <c r="E106" s="1" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="106" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A106" s="1" t="s">
+    <row r="107" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A107" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="E106" s="1" t="s">
+      <c r="E107" s="1" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="107" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A107" s="1" t="s">
+    <row r="108" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A108" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E107" s="1" t="s">
+      <c r="E108" s="1" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="108" spans="1:5" ht="64" x14ac:dyDescent="0.2">
-      <c r="A108" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E108" s="1" t="s">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A109" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E109" s="1" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="109" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A109" s="1" t="s">
+    <row r="110" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A110" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="E109" s="1" t="s">
+      <c r="E110" s="1" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="110" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A110" s="1" t="s">
+    <row r="111" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A111" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="E110" s="1" t="s">
+      <c r="E111" s="1" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="111" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A111" s="1" t="s">
+    <row r="112" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+      <c r="A112" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E111" s="1" t="s">
+      <c r="E112" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A113" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E113" s="1" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="112" spans="1:5" ht="64" x14ac:dyDescent="0.2">
-      <c r="A112" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="E112" s="1" t="s">
+    <row r="114" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A114" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E114" s="1" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="113" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A113" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="E113" s="1" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" ht="80" x14ac:dyDescent="0.2">
-      <c r="A114" s="1" t="s">
+    <row r="115" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+      <c r="A115" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E114" s="1" t="s">
+      <c r="E115" s="1" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="115" spans="1:5" ht="64" x14ac:dyDescent="0.2">
-      <c r="A115" s="1" t="s">
+    <row r="116" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A116" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E115" s="1" t="s">
+      <c r="E116" s="1" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="116" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A116" s="1" t="s">
+    <row r="117" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A117" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="E116" s="1" t="s">
+      <c r="E117" s="1" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="117" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A117" s="1" t="s">
+    <row r="118" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A118" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E117" s="1" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A118" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+    </row>
+    <row r="119" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A119" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="120" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A120" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="121" spans="1:5" ht="80" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A121" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Started transferring classifications into subclassifications
Former-commit-id: df151597dbf4ba5564d277771552906e78a4dfa2
</commit_message>
<xml_diff>
--- a/Classifications/Vid_1_Morgan_Proofread_Calvin.xlsx
+++ b/Classifications/Vid_1_Morgan_Proofread_Calvin.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iowa-my.sharepoint.com/personal/krector_uiowa_edu/Documents/aerobictextreview/Classifications/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iowa-my.sharepoint.com/personal/cjskalla_uiowa_edu/Documents/Documents/aerobictextreview/Classifications/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="8_{C9BA6B64-C06B-1E42-B451-CADF41EFF0DC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B2E9C343-AAFF-4FBC-A900-215CCE2C591A}"/>
+  <xr:revisionPtr revIDLastSave="157" documentId="8_{C9BA6B64-C06B-1E42-B451-CADF41EFF0DC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{D695BA8C-A46F-4033-9900-9FB52CDE5DDE}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3375" yWindow="3975" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="258">
   <si>
     <t>hey everybody it's your personal trainer coach Kozak here from HASFIT.</t>
   </si>
@@ -929,6 +929,12 @@
   </si>
   <si>
     <t>we're getting ready we're starting with the row</t>
+  </si>
+  <si>
+    <t>we're going to finish up with some ABS</t>
+  </si>
+  <si>
+    <t>we don't have much left we got what about up one more exercise one more after this one</t>
   </si>
 </sst>
 </file>
@@ -944,7 +950,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -969,8 +975,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -978,11 +996,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -995,6 +1028,18 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1277,26 +1322,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomLeft" activeCell="A121" sqref="A119:A121"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.6328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="33.453125" customWidth="1"/>
-    <col min="4" max="4" width="8.6328125" customWidth="1"/>
-    <col min="5" max="5" width="45.453125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="3.453125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="15.1796875" customWidth="1"/>
-    <col min="8" max="8" width="2.36328125" customWidth="1"/>
-    <col min="9" max="9" width="24.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="1.81640625" customWidth="1"/>
-    <col min="11" max="11" width="35.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="33.42578125" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" customWidth="1"/>
+    <col min="5" max="5" width="45.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="3.42578125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" customWidth="1"/>
+    <col min="8" max="8" width="2.42578125" customWidth="1"/>
+    <col min="9" max="9" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="1.85546875" customWidth="1"/>
+    <col min="11" max="11" width="35.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>144</v>
       </c>
@@ -1322,15 +1367,15 @@
         <v>146</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="6" t="s">
         <v>111</v>
       </c>
       <c r="D2" s="1"/>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="6" t="s">
         <v>139</v>
       </c>
       <c r="G2" s="4" t="s">
@@ -1343,12 +1388,12 @@
         <v>112</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="C3" s="1" t="s">
+    <row r="3" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="C3" s="6" t="s">
         <v>120</v>
       </c>
       <c r="D3" s="1"/>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="6" t="s">
         <v>66</v>
       </c>
       <c r="G3" s="4" t="s">
@@ -1361,11 +1406,11 @@
         <v>254</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="87" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="6" t="s">
         <v>140</v>
       </c>
       <c r="G4" s="4" t="s">
@@ -1374,12 +1419,15 @@
       <c r="I4" s="5" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
+      <c r="K4" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="6" t="s">
         <v>147</v>
       </c>
       <c r="G5" s="4" t="s">
@@ -1388,935 +1436,986 @@
       <c r="I5" s="4" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+      <c r="K5" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="6" t="s">
         <v>130</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
+      <c r="K6" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="6" t="s">
         <v>122</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>123</v>
       </c>
       <c r="I7" s="4" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
+      <c r="K7" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="6" t="s">
         <v>137</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>185</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
+      <c r="K8" s="6" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="6" t="s">
         <v>118</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>249</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="87" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="6" t="s">
         <v>109</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>70</v>
       </c>
       <c r="I10" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="6" t="s">
         <v>18</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>210</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="6" t="s">
         <v>133</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>124</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="6" t="s">
         <v>248</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>171</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="C14" s="1" t="s">
+    <row r="14" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="C14" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" s="6" t="s">
         <v>181</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="C15" s="1" t="s">
+    <row r="15" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="C15" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" s="6" t="s">
         <v>184</v>
       </c>
       <c r="I15" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" s="6" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
+      <c r="I16" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" s="6" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="C18" s="1" t="s">
+      <c r="I17" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="C18" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" s="6" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
+      <c r="I18" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E20" s="1" t="s">
+      <c r="I19" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="E20" s="6" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E21" s="1" t="s">
+      <c r="I20" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E21" s="6" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A22" s="1" t="s">
+    <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E22" s="6" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A23" s="1" t="s">
+    <row r="23" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E23" s="6" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E24" s="1" t="s">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E24" s="6" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A25" s="1" t="s">
+    <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E25" s="6" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="1" t="s">
+    <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E26" s="6" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="1" t="s">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E27" s="6" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A28" s="1" t="s">
+    <row r="28" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E28" s="6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A29" s="1" t="s">
+    <row r="29" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E29" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="1" t="s">
+    <row r="30" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E30" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="1" t="s">
+    <row r="31" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E31" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="1" t="s">
+    <row r="32" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E32" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A33" s="1" t="s">
+    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E33" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A34" s="1" t="s">
+    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A35" s="1" t="s">
+    <row r="35" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="E35" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A36" s="1" t="s">
+    <row r="36" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="E36" s="6" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A37" s="1" t="s">
+    <row r="37" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="E37" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A38" s="1" t="s">
+    <row r="38" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="E38" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A39" s="1" t="s">
+    <row r="39" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="E39" s="6" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="1" t="s">
+    <row r="40" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="E40" s="6" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="E41" s="1" t="s">
+    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="E41" s="6" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E42" s="1" t="s">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E42" s="6" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A43" s="1" t="s">
+    <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="E43" s="6" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A44" s="1" t="s">
+    <row r="44" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="E44" s="1" t="s">
+      <c r="E44" s="6" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A45" s="1" t="s">
+    <row r="45" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="E45" s="6" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="E46" s="1" t="s">
+    <row r="46" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="E46" s="6" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A47" s="1" t="s">
+    <row r="47" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A47" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E47" s="1" t="s">
+      <c r="E47" s="6" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A48" s="1" t="s">
+    <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="E48" s="1" t="s">
+      <c r="E48" s="6" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A49" s="1" t="s">
+    <row r="49" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A49" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="E49" s="6" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A50" s="1" t="s">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="E51" s="1" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A52" s="1" t="s">
+    <row r="52" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" s="6" t="s">
         <v>29</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A53" s="1" t="s">
+    <row r="53" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A53" s="6" t="s">
         <v>30</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A54" s="1" t="s">
+    <row r="54" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54" s="6" t="s">
         <v>32</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A55" s="1" t="s">
+    <row r="55" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A55" s="6" t="s">
         <v>35</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A56" s="1" t="s">
+    <row r="56" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56" s="6" t="s">
         <v>37</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A57" s="1" t="s">
+    <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" s="6" t="s">
         <v>38</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E58" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A59" s="1" t="s">
+    <row r="59" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" s="6" t="s">
         <v>41</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A60" s="1" t="s">
+    <row r="60" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A60" s="6" t="s">
         <v>43</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A61" s="1" t="s">
+    <row r="61" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61" s="6" t="s">
         <v>45</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A62" s="1" t="s">
+    <row r="62" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A62" s="6" t="s">
         <v>46</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A63" s="1" t="s">
+    <row r="63" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A63" s="6" t="s">
         <v>47</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A64" s="1" t="s">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A65" s="1" t="s">
+    <row r="65" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A65" s="6" t="s">
         <v>51</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E66" s="1" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A67" s="1" t="s">
+    <row r="67" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A67" s="6" t="s">
         <v>53</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A68" s="1" t="s">
+    <row r="68" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A68" s="6" t="s">
         <v>54</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A69" s="1" t="s">
+    <row r="69" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A69" s="6" t="s">
         <v>56</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A70" s="1" t="s">
+    <row r="70" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A70" s="6" t="s">
         <v>55</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A71" s="1" t="s">
+    <row r="71" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A71" s="6" t="s">
         <v>57</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A72" s="1" t="s">
+    <row r="72" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A72" s="6" t="s">
         <v>50</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A73" s="1" t="s">
+    <row r="73" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A73" s="6" t="s">
         <v>58</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A74" s="1" t="s">
+    <row r="74" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A74" s="6" t="s">
         <v>214</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="87" x14ac:dyDescent="0.35">
-      <c r="A75" s="1" t="s">
+    <row r="75" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A75" s="6" t="s">
         <v>213</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A76" s="1" t="s">
+    <row r="76" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A76" s="6" t="s">
         <v>64</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A77" s="1" t="s">
+    <row r="77" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A77" s="6" t="s">
         <v>216</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A78" s="1" t="s">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="6" t="s">
         <v>68</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A79" s="1" t="s">
+    <row r="79" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A79" s="6" t="s">
         <v>215</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="80" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A80" s="1" t="s">
+    <row r="80" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A80" s="6" t="s">
         <v>217</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A81" s="1" t="s">
+    <row r="81" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A81" s="6" t="s">
         <v>218</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A82" s="1" t="s">
+    <row r="82" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A82" s="6" t="s">
         <v>219</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="83" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A83" s="1" t="s">
+    <row r="83" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A83" s="6" t="s">
         <v>71</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="84" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A84" s="1" t="s">
+    <row r="84" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A84" s="6" t="s">
         <v>220</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A85" s="1" t="s">
+    <row r="85" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A85" s="6" t="s">
         <v>72</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A86" s="1" t="s">
+    <row r="86" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A86" s="6" t="s">
         <v>73</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="87" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A87" s="1" t="s">
+    <row r="87" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A87" s="6" t="s">
         <v>221</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="88" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A88" s="1" t="s">
+    <row r="88" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A88" s="6" t="s">
         <v>222</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="89" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A89" s="1" t="s">
+    <row r="89" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A89" s="6" t="s">
         <v>223</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="90" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A90" s="1" t="s">
+    <row r="90" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A90" s="6" t="s">
         <v>74</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="91" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A91" s="1" t="s">
+    <row r="91" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A91" s="6" t="s">
         <v>75</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="92" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A92" s="1" t="s">
+    <row r="92" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A92" s="6" t="s">
         <v>76</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="93" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A93" s="1" t="s">
+    <row r="93" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A93" s="6" t="s">
         <v>77</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="94" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A94" s="1" t="s">
+    <row r="94" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A94" s="6" t="s">
         <v>78</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="95" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A95" s="1" t="s">
+    <row r="95" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A95" s="6" t="s">
         <v>79</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="96" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A96" s="1" t="s">
+    <row r="96" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A96" s="6" t="s">
         <v>80</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="97" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A97" s="1" t="s">
+    <row r="97" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A97" s="6" t="s">
         <v>81</v>
       </c>
       <c r="E97" s="1" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="98" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A98" s="1" t="s">
+    <row r="98" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A98" s="6" t="s">
         <v>82</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="99" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A99" s="1" t="s">
+    <row r="99" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A99" s="9" t="s">
         <v>83</v>
       </c>
       <c r="E99" s="1" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="100" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A100" s="1" t="s">
+    <row r="100" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A100" s="6" t="s">
         <v>84</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="101" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A101" s="1" t="s">
+    <row r="101" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A101" s="6" t="s">
         <v>85</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="102" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A102" s="1" t="s">
+    <row r="102" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A102" s="6" t="s">
         <v>86</v>
       </c>
       <c r="E102" s="1" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="103" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A103" s="1" t="s">
+    <row r="103" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A103" s="6" t="s">
         <v>87</v>
       </c>
       <c r="E103" s="1" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A104" s="1" t="s">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" s="6" t="s">
         <v>89</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="105" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A105" s="1" t="s">
+    <row r="105" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A105" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="106" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A106" s="1" t="s">
+    <row r="106" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A106" s="6" t="s">
         <v>92</v>
       </c>
       <c r="E106" s="1" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="107" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A107" s="1" t="s">
+    <row r="107" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A107" s="6" t="s">
         <v>93</v>
       </c>
       <c r="E107" s="1" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="108" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A108" s="1" t="s">
+    <row r="108" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A108" s="6" t="s">
         <v>94</v>
       </c>
       <c r="E108" s="1" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A109" s="1" t="s">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" s="6" t="s">
         <v>96</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="110" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A110" s="1" t="s">
+    <row r="110" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A110" s="6" t="s">
         <v>97</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="111" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A111" s="1" t="s">
+    <row r="111" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A111" s="6" t="s">
         <v>98</v>
       </c>
       <c r="E111" s="1" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="112" spans="1:5" ht="87" x14ac:dyDescent="0.35">
-      <c r="A112" s="1" t="s">
+    <row r="112" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A112" s="6" t="s">
         <v>99</v>
       </c>
       <c r="E112" s="1" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="113" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A113" s="1" t="s">
+    <row r="113" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A113" s="6" t="s">
         <v>100</v>
       </c>
       <c r="E113" s="1" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="114" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A114" s="1" t="s">
+    <row r="114" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A114" s="6" t="s">
         <v>101</v>
       </c>
       <c r="E114" s="1" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="115" spans="1:5" ht="87" x14ac:dyDescent="0.35">
-      <c r="A115" s="1" t="s">
+    <row r="115" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A115" s="6" t="s">
         <v>102</v>
       </c>
       <c r="E115" s="1" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="116" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A116" s="1" t="s">
+    <row r="116" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A116" s="6" t="s">
         <v>103</v>
       </c>
       <c r="E116" s="1" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="117" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A117" s="1" t="s">
+    <row r="117" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A117" s="6" t="s">
         <v>104</v>
       </c>
       <c r="E117" s="1" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="118" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A118" s="1" t="s">
+    <row r="118" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A118" s="6" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="119" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A119" s="1" t="s">
+    <row r="119" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A119" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="120" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A120" s="1" t="s">
+    <row r="120" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A120" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="121" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A121" s="1" t="s">
+    <row r="121" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A121" s="6" t="s">
         <v>170</v>
       </c>
     </row>

</xml_diff>